<commit_message>
Fixes bug with superstructure db export
The production flows were not listed in the scenario difference file.
Also, in the case of losses, those were replacing the production flow values, leading to wrong results.
Now losses are subtracted from the production flow value (which is typically 1).
For example, for electricity markets, the output flow is no longer 1 kWh but 1 - loss.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-synfuels-from-FT-from-electrolysis.xlsx
+++ b/premise/data/additional_inventories/lci-synfuels-from-FT-from-electrolysis.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="FT fuel - Diesel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateCount="15" iterateDelta="0.01"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="132">
   <si>
     <t>Activity</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>Diesel, synthetic</t>
-  </si>
-  <si>
-    <t>Lubricating oil production, synthetic, Fischer Tropsch process, economic allocation</t>
   </si>
   <si>
     <t>Lubricating oil, synthetic</t>
@@ -391,28 +388,34 @@
     <t>wastewater, average</t>
   </si>
   <si>
-    <t>kerosene</t>
-  </si>
-  <si>
     <t>diesel, synthetic, vehicle grade</t>
   </si>
   <si>
-    <t>Kerosene, synthetic, from electrolysis-based hydrogen, economic allocation, at fuelling station</t>
-  </si>
-  <si>
-    <t>Diesel, synthetic, from electrolysis-based hydrogen, economic allocation, at fuelling station</t>
-  </si>
-  <si>
-    <t>Kerosene, synthetic, from electrolysis-based hydrogen, energy allocation, at fuelling station</t>
-  </si>
-  <si>
-    <t>Diesel, synthetic, from electrolysis-based hydrogen, energy allocation, at fuelling station</t>
-  </si>
-  <si>
     <t>treatment of wastewater, average, capacity 1E9l/year</t>
   </si>
   <si>
     <t>synfuel from electrolysis</t>
+  </si>
+  <si>
+    <t>lubricating oil production, synthetic, Fischer Tropsch process, economic allocation</t>
+  </si>
+  <si>
+    <t>lubricating oil, synthetic</t>
+  </si>
+  <si>
+    <t>kerosene production, synthetic, from electrolysis-based hydrogen, economic allocation, at fuelling station</t>
+  </si>
+  <si>
+    <t>kerosene, synthetic</t>
+  </si>
+  <si>
+    <t>diesel production, synthetic, from electrolysis-based hydrogen, economic allocation, at fuelling station</t>
+  </si>
+  <si>
+    <t>kerosene production, synthetic, from electrolysis-based hydrogen, energy allocation, at fuelling station</t>
+  </si>
+  <si>
+    <t>diesel production, synthetic, from electrolysis-based hydrogen, energy allocation, at fuelling station</t>
   </si>
 </sst>
 </file>
@@ -839,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K654"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,7 +858,7 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -866,7 +869,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -882,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>41</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -914,15 +917,15 @@
         <v>9</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -961,7 +964,7 @@
     </row>
     <row r="13" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="B13" s="15">
         <v>1</v>
@@ -976,10 +979,10 @@
         <v>15</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>16</v>
@@ -1005,7 +1008,7 @@
         <v>17</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1050,7 +1053,7 @@
     </row>
     <row r="17" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="17">
         <v>6.7000000000000001E-12</v>
@@ -1065,10 +1068,10 @@
         <v>18</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1096,7 +1099,7 @@
     </row>
     <row r="19" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="15">
         <v>7.06</v>
@@ -1122,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1146,7 +1149,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1190,13 +1193,13 @@
         <v>3</v>
       </c>
       <c r="G28" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="I28" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="J28" s="15" t="s">
         <v>9</v>
@@ -1207,7 +1210,7 @@
     </row>
     <row r="29" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B29" s="16">
         <v>1</v>
@@ -1228,15 +1231,15 @@
         <v>100</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K29" s="18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="16">
         <v>1.00057</v>
@@ -1256,7 +1259,7 @@
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
       <c r="K30" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1286,13 +1289,13 @@
     </row>
     <row r="32" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" s="21">
         <v>1.8499999999999999E-5</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>6</v>
@@ -1306,18 +1309,18 @@
       <c r="I32" s="16"/>
       <c r="J32" s="16"/>
       <c r="K32" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="21">
         <v>5.8399999999999999E-4</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>20</v>
@@ -1331,12 +1334,12 @@
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
       <c r="K33" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B34" s="21">
         <v>1.04E-10</v>
@@ -1356,18 +1359,18 @@
       <c r="I34" s="16"/>
       <c r="J34" s="16"/>
       <c r="K34" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B35" s="21">
         <v>-6.2700000000000001E-6</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>6</v>
@@ -1381,18 +1384,18 @@
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
       <c r="K35" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B36" s="21">
         <v>-5.0000000000000002E-5</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" s="20" t="s">
         <v>25</v>
@@ -1406,18 +1409,18 @@
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="21">
         <v>6.8900000000000005E-4</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>6</v>
@@ -1431,21 +1434,21 @@
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
       <c r="K37" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="16">
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16" t="s">
@@ -1456,12 +1459,12 @@
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="16">
         <v>3.2599999999999997E-2</v>
@@ -1470,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E39" s="16"/>
       <c r="F39" s="16" t="s">
@@ -1481,18 +1484,18 @@
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B40" s="21">
         <v>-6.8899999999999999E-7</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D40" s="16" t="s">
         <v>25</v>
@@ -1506,7 +1509,7 @@
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1519,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1543,7 +1546,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1587,13 +1590,13 @@
         <v>3</v>
       </c>
       <c r="G49" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H49" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H49" s="15" t="s">
+      <c r="I49" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="J49" s="15" t="s">
         <v>9</v>
@@ -1604,7 +1607,7 @@
     </row>
     <row r="50" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="16" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B50" s="16">
         <v>1</v>
@@ -1625,15 +1628,15 @@
         <v>100</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K50" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B51" s="16">
         <v>1.00057</v>
@@ -1683,13 +1686,13 @@
     </row>
     <row r="53" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="16">
         <v>-1.6799999999999999E-4</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D53" s="16" t="s">
         <v>6</v>
@@ -1703,18 +1706,18 @@
       <c r="I53" s="16"/>
       <c r="J53" s="16"/>
       <c r="K53" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B54" s="21">
         <v>5.8399999999999999E-4</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D54" s="16" t="s">
         <v>20</v>
@@ -1728,12 +1731,12 @@
       <c r="I54" s="16"/>
       <c r="J54" s="16"/>
       <c r="K54" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B55" s="21">
         <v>2.5999999999999998E-10</v>
@@ -1753,18 +1756,18 @@
       <c r="I55" s="16"/>
       <c r="J55" s="16"/>
       <c r="K55" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B56" s="21">
         <v>-6.2700000000000001E-6</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D56" s="16" t="s">
         <v>6</v>
@@ -1778,18 +1781,18 @@
       <c r="I56" s="16"/>
       <c r="J56" s="16"/>
       <c r="K56" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B57" s="21">
         <v>-7.4999999999999993E-5</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>25</v>
@@ -1803,18 +1806,18 @@
       <c r="I57" s="16"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B58" s="21">
         <v>6.8900000000000005E-4</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D58" s="16" t="s">
         <v>6</v>
@@ -1828,21 +1831,21 @@
       <c r="I58" s="16"/>
       <c r="J58" s="16"/>
       <c r="K58" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B59" s="16">
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="C59" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E59" s="16"/>
       <c r="F59" s="16" t="s">
@@ -1853,12 +1856,12 @@
       <c r="I59" s="16"/>
       <c r="J59" s="16"/>
       <c r="K59" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60" s="16">
         <v>3.2599999999999997E-2</v>
@@ -1867,7 +1870,7 @@
         <v>8</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E60" s="16"/>
       <c r="F60" s="16" t="s">
@@ -1878,18 +1881,18 @@
       <c r="I60" s="16"/>
       <c r="J60" s="16"/>
       <c r="K60" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B61" s="21">
         <v>-6.8899999999999999E-7</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D61" s="16" t="s">
         <v>25</v>
@@ -1903,7 +1906,7 @@
       <c r="I61" s="16"/>
       <c r="J61" s="16"/>
       <c r="K61" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -1916,7 +1919,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1940,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1984,13 +1987,13 @@
         <v>3</v>
       </c>
       <c r="G70" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H70" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H70" s="15" t="s">
+      <c r="I70" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="I70" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="J70" s="15" t="s">
         <v>9</v>
@@ -2001,7 +2004,7 @@
     </row>
     <row r="71" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="16" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B71" s="16">
         <v>1</v>
@@ -2022,15 +2025,15 @@
         <v>100</v>
       </c>
       <c r="J71" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K71" s="18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B72" s="16">
         <v>1.00057</v>
@@ -2050,7 +2053,7 @@
       <c r="I72" s="16"/>
       <c r="J72" s="16"/>
       <c r="K72" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2080,13 +2083,13 @@
     </row>
     <row r="74" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B74" s="21">
         <v>1.8499999999999999E-5</v>
       </c>
       <c r="C74" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D74" s="16" t="s">
         <v>6</v>
@@ -2100,18 +2103,18 @@
       <c r="I74" s="16"/>
       <c r="J74" s="16"/>
       <c r="K74" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B75" s="21">
         <v>5.8399999999999999E-4</v>
       </c>
       <c r="C75" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75" s="16" t="s">
         <v>20</v>
@@ -2125,12 +2128,12 @@
       <c r="I75" s="16"/>
       <c r="J75" s="16"/>
       <c r="K75" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B76" s="21">
         <v>1.04E-10</v>
@@ -2150,18 +2153,18 @@
       <c r="I76" s="16"/>
       <c r="J76" s="16"/>
       <c r="K76" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B77" s="21">
         <v>-6.2700000000000001E-6</v>
       </c>
       <c r="C77" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D77" s="16" t="s">
         <v>6</v>
@@ -2175,18 +2178,18 @@
       <c r="I77" s="16"/>
       <c r="J77" s="16"/>
       <c r="K77" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B78" s="21">
         <v>-5.0000000000000002E-5</v>
       </c>
       <c r="C78" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>25</v>
@@ -2200,18 +2203,18 @@
       <c r="I78" s="16"/>
       <c r="J78" s="16"/>
       <c r="K78" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B79" s="21">
         <v>6.8900000000000005E-4</v>
       </c>
       <c r="C79" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D79" s="16" t="s">
         <v>6</v>
@@ -2225,21 +2228,21 @@
       <c r="I79" s="16"/>
       <c r="J79" s="16"/>
       <c r="K79" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B80" s="16">
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D80" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E80" s="16"/>
       <c r="F80" s="16" t="s">
@@ -2250,12 +2253,12 @@
       <c r="I80" s="16"/>
       <c r="J80" s="16"/>
       <c r="K80" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B81" s="16">
         <v>3.2599999999999997E-2</v>
@@ -2264,7 +2267,7 @@
         <v>8</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E81" s="16"/>
       <c r="F81" s="16" t="s">
@@ -2275,18 +2278,18 @@
       <c r="I81" s="16"/>
       <c r="J81" s="16"/>
       <c r="K81" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B82" s="21">
         <v>-6.8899999999999999E-7</v>
       </c>
       <c r="C82" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D82" s="16" t="s">
         <v>25</v>
@@ -2300,7 +2303,7 @@
       <c r="I82" s="16"/>
       <c r="J82" s="16"/>
       <c r="K82" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2313,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2337,7 +2340,7 @@
         <v>2</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2381,13 +2384,13 @@
         <v>3</v>
       </c>
       <c r="G91" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="H91" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="H91" s="15" t="s">
+      <c r="I91" s="15" t="s">
         <v>102</v>
-      </c>
-      <c r="I91" s="15" t="s">
-        <v>103</v>
       </c>
       <c r="J91" s="15" t="s">
         <v>9</v>
@@ -2398,7 +2401,7 @@
     </row>
     <row r="92" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="16" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B92" s="16">
         <v>1</v>
@@ -2419,15 +2422,15 @@
         <v>100</v>
       </c>
       <c r="J92" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K92" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B93" s="16">
         <v>1.00057</v>
@@ -2477,13 +2480,13 @@
     </row>
     <row r="95" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B95" s="16">
         <v>-1.6799999999999999E-4</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D95" s="16" t="s">
         <v>6</v>
@@ -2497,18 +2500,18 @@
       <c r="I95" s="16"/>
       <c r="J95" s="16"/>
       <c r="K95" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B96" s="21">
         <v>5.8399999999999999E-4</v>
       </c>
       <c r="C96" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D96" s="16" t="s">
         <v>20</v>
@@ -2522,12 +2525,12 @@
       <c r="I96" s="16"/>
       <c r="J96" s="16"/>
       <c r="K96" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A97" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B97" s="21">
         <v>2.5999999999999998E-10</v>
@@ -2547,18 +2550,18 @@
       <c r="I97" s="16"/>
       <c r="J97" s="16"/>
       <c r="K97" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A98" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B98" s="21">
         <v>-6.2700000000000001E-6</v>
       </c>
       <c r="C98" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D98" s="16" t="s">
         <v>6</v>
@@ -2572,18 +2575,18 @@
       <c r="I98" s="16"/>
       <c r="J98" s="16"/>
       <c r="K98" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A99" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B99" s="21">
         <v>-7.4999999999999993E-5</v>
       </c>
       <c r="C99" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D99" s="20" t="s">
         <v>25</v>
@@ -2597,18 +2600,18 @@
       <c r="I99" s="16"/>
       <c r="J99" s="16"/>
       <c r="K99" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B100" s="21">
         <v>6.8900000000000005E-4</v>
       </c>
       <c r="C100" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D100" s="16" t="s">
         <v>6</v>
@@ -2622,21 +2625,21 @@
       <c r="I100" s="16"/>
       <c r="J100" s="16"/>
       <c r="K100" s="16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A101" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B101" s="16">
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="C101" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
@@ -2647,12 +2650,12 @@
       <c r="I101" s="16"/>
       <c r="J101" s="16"/>
       <c r="K101" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="102" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A102" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B102" s="16">
         <v>3.2599999999999997E-2</v>
@@ -2661,7 +2664,7 @@
         <v>8</v>
       </c>
       <c r="D102" s="16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E102" s="16"/>
       <c r="F102" s="16" t="s">
@@ -2672,18 +2675,18 @@
       <c r="I102" s="16"/>
       <c r="J102" s="16"/>
       <c r="K102" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="16" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B103" s="21">
         <v>-6.8899999999999999E-7</v>
       </c>
       <c r="C103" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D103" s="16" t="s">
         <v>25</v>
@@ -2697,7 +2700,7 @@
       <c r="I103" s="16"/>
       <c r="J103" s="16"/>
       <c r="K103" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:11" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2710,7 +2713,7 @@
         <v>0</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="106" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2726,7 +2729,7 @@
         <v>2</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="108" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2758,15 +2761,15 @@
         <v>9</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="112" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B112" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="113" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -2805,7 +2808,7 @@
     </row>
     <row r="115" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B115" s="15">
         <v>1</v>
@@ -2820,10 +2823,10 @@
         <v>15</v>
       </c>
       <c r="G115" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H115" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I115" s="15" t="s">
         <v>16</v>
@@ -2849,7 +2852,7 @@
         <v>17</v>
       </c>
       <c r="H116" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="117" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2894,7 +2897,7 @@
     </row>
     <row r="119" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B119" s="17">
         <v>6.7000000000000001E-12</v>
@@ -2909,10 +2912,10 @@
         <v>18</v>
       </c>
       <c r="G119" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H119" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="120" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2940,7 +2943,7 @@
     </row>
     <row r="121" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B121" s="15">
         <v>2</v>
@@ -2949,7 +2952,7 @@
         <v>6</v>
       </c>
       <c r="E121" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F121" s="15" t="s">
         <v>22</v>
@@ -2964,7 +2967,7 @@
         <v>0</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="124" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -2980,7 +2983,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="126" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3012,15 +3015,15 @@
         <v>9</v>
       </c>
       <c r="B129" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="130" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B130" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B130" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="131" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3059,7 +3062,7 @@
     </row>
     <row r="133" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B133" s="15">
         <v>1</v>
@@ -3074,10 +3077,10 @@
         <v>15</v>
       </c>
       <c r="G133" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H133" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="134" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3100,7 +3103,7 @@
         <v>17</v>
       </c>
       <c r="H134" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="135" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3145,7 +3148,7 @@
     </row>
     <row r="137" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B137" s="17">
         <v>6.7000000000000001E-12</v>
@@ -3160,10 +3163,10 @@
         <v>18</v>
       </c>
       <c r="G137" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H137" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="138" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3191,7 +3194,7 @@
     </row>
     <row r="139" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B139" s="15">
         <v>2.48</v>
@@ -3200,7 +3203,7 @@
         <v>6</v>
       </c>
       <c r="E139" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F139" s="15" t="s">
         <v>22</v>
@@ -3215,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="142" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3263,15 +3266,15 @@
         <v>9</v>
       </c>
       <c r="B147" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="148" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B148" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B148" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="149" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3310,7 +3313,7 @@
     </row>
     <row r="151" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B151" s="15">
         <v>1</v>
@@ -3328,7 +3331,7 @@
         <v>39</v>
       </c>
       <c r="H151" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I151" s="15" t="s">
         <v>16</v>
@@ -3354,7 +3357,7 @@
         <v>17</v>
       </c>
       <c r="H152" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="153" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3399,7 +3402,7 @@
     </row>
     <row r="155" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B155" s="17">
         <v>6.7000000000000001E-12</v>
@@ -3414,10 +3417,10 @@
         <v>18</v>
       </c>
       <c r="G155" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H155" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3445,7 +3448,7 @@
     </row>
     <row r="157" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B157" s="15">
         <v>1.82</v>
@@ -3454,7 +3457,7 @@
         <v>6</v>
       </c>
       <c r="E157" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F157" s="15" t="s">
         <v>22</v>
@@ -3469,7 +3472,7 @@
         <v>0</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="160" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3485,7 +3488,7 @@
         <v>2</v>
       </c>
       <c r="B161" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="162" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3517,15 +3520,15 @@
         <v>9</v>
       </c>
       <c r="B165" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="166" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B166" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B166" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="167" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3564,7 +3567,7 @@
     </row>
     <row r="169" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B169" s="15">
         <v>1</v>
@@ -3579,10 +3582,10 @@
         <v>15</v>
       </c>
       <c r="G169" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H169" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I169" s="15" t="s">
         <v>16</v>
@@ -3608,7 +3611,7 @@
         <v>17</v>
       </c>
       <c r="H170" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3653,7 +3656,7 @@
     </row>
     <row r="173" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B173" s="17">
         <v>6.7000000000000001E-12</v>
@@ -3668,10 +3671,10 @@
         <v>18</v>
       </c>
       <c r="G173" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H173" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="174" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3699,7 +3702,7 @@
     </row>
     <row r="175" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B175" s="15">
         <v>0.13</v>
@@ -3725,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="B177" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="178" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3741,7 +3744,7 @@
         <v>2</v>
       </c>
       <c r="B179" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="180" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3773,15 +3776,15 @@
         <v>9</v>
       </c>
       <c r="B183" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="184" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B184" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B184" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="185" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -3820,7 +3823,7 @@
     </row>
     <row r="187" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B187" s="15">
         <v>1</v>
@@ -3835,10 +3838,10 @@
         <v>15</v>
       </c>
       <c r="G187" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H187" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I187" s="15" t="s">
         <v>16</v>
@@ -3864,7 +3867,7 @@
         <v>17</v>
       </c>
       <c r="H188" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="189" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3909,7 +3912,7 @@
     </row>
     <row r="191" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B191" s="17">
         <v>6.7000000000000001E-12</v>
@@ -3924,10 +3927,10 @@
         <v>18</v>
       </c>
       <c r="G191" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H191" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="192" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3955,7 +3958,7 @@
     </row>
     <row r="193" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B193" s="15">
         <v>0.22</v>
@@ -3979,7 +3982,7 @@
         <v>0</v>
       </c>
       <c r="B195" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="196" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -3995,7 +3998,7 @@
         <v>2</v>
       </c>
       <c r="B197" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="198" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4027,15 +4030,15 @@
         <v>9</v>
       </c>
       <c r="B201" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="202" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B202" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B202" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="203" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4074,7 +4077,7 @@
     </row>
     <row r="205" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B205" s="15">
         <v>1</v>
@@ -4089,10 +4092,10 @@
         <v>15</v>
       </c>
       <c r="G205" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H205" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="206" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4115,7 +4118,7 @@
         <v>17</v>
       </c>
       <c r="H206" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="207" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4160,7 +4163,7 @@
     </row>
     <row r="209" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B209" s="17">
         <v>6.7000000000000001E-12</v>
@@ -4175,10 +4178,10 @@
         <v>18</v>
       </c>
       <c r="G209" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H209" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="210" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4206,7 +4209,7 @@
     </row>
     <row r="211" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B211" s="15">
         <v>0.19</v>
@@ -4215,7 +4218,7 @@
         <v>6</v>
       </c>
       <c r="E211" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F211" s="15" t="s">
         <v>22</v>
@@ -4230,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="B213" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="214" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4278,15 +4281,15 @@
         <v>9</v>
       </c>
       <c r="B219" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="220" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B220" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B220" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="221" spans="1:9" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4325,7 +4328,7 @@
     </row>
     <row r="223" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B223" s="15">
         <v>1</v>
@@ -4343,7 +4346,7 @@
         <v>39</v>
       </c>
       <c r="H223" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I223" s="15" t="s">
         <v>16</v>
@@ -4369,7 +4372,7 @@
         <v>17</v>
       </c>
       <c r="H224" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="225" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4414,7 +4417,7 @@
     </row>
     <row r="227" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B227" s="17">
         <v>6.7000000000000001E-12</v>
@@ -4429,10 +4432,10 @@
         <v>18</v>
       </c>
       <c r="G227" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H227" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="228" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4460,7 +4463,7 @@
     </row>
     <row r="229" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B229" s="15">
         <v>0.06</v>
@@ -4469,7 +4472,7 @@
         <v>6</v>
       </c>
       <c r="E229" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F229" s="15" t="s">
         <v>22</v>
@@ -4537,10 +4540,10 @@
     </row>
     <row r="238" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A238" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B238" s="15" t="s">
         <v>43</v>
-      </c>
-      <c r="B238" s="15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="239" spans="1:8" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4608,7 +4611,7 @@
         <v>18</v>
       </c>
       <c r="G242" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="243" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4810,7 +4813,7 @@
         <v>18</v>
       </c>
       <c r="G258" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="259" spans="1:7" s="15" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4830,12 +4833,12 @@
         <v>18</v>
       </c>
       <c r="G259" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="260" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A260" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B260" s="17">
         <v>1.9300000000000002E-9</v>
@@ -4850,7 +4853,7 @@
         <v>18</v>
       </c>
       <c r="G260" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="261" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -4863,7 +4866,7 @@
         <v>0</v>
       </c>
       <c r="B262" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="263" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4879,7 +4882,7 @@
         <v>2</v>
       </c>
       <c r="B264" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="265" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4911,15 +4914,15 @@
         <v>9</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="269" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A269" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B269" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B269" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="270" spans="1:7" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -4952,7 +4955,7 @@
     </row>
     <row r="272" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A272" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B272" s="8">
         <v>1</v>
@@ -4967,18 +4970,18 @@
         <v>15</v>
       </c>
       <c r="G272" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="273" spans="1:7" ht="15" x14ac:dyDescent="0.35">
       <c r="A273" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B273" s="3">
         <v>345000</v>
       </c>
       <c r="C273" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D273" t="s">
         <v>25</v>
@@ -4987,7 +4990,7 @@
         <v>18</v>
       </c>
       <c r="G273" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
@@ -5012,7 +5015,7 @@
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B275" s="3">
         <v>7200000</v>
@@ -5027,38 +5030,38 @@
         <v>18</v>
       </c>
       <c r="G275" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B276" s="3">
         <v>-828000000</v>
       </c>
       <c r="C276" t="s">
+        <v>77</v>
+      </c>
+      <c r="D276" t="s">
+        <v>6</v>
+      </c>
+      <c r="F276" t="s">
+        <v>18</v>
+      </c>
+      <c r="G276" t="s">
         <v>78</v>
-      </c>
-      <c r="D276" t="s">
-        <v>6</v>
-      </c>
-      <c r="F276" t="s">
-        <v>18</v>
-      </c>
-      <c r="G276" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A277" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B277" s="3">
         <v>-14400000</v>
       </c>
       <c r="C277" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D277" t="s">
         <v>6</v>
@@ -5067,21 +5070,21 @@
         <v>18</v>
       </c>
       <c r="G277" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A278" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B278" s="3">
         <v>1120000</v>
       </c>
       <c r="D278" t="s">
+        <v>82</v>
+      </c>
+      <c r="E278" t="s">
         <v>83</v>
-      </c>
-      <c r="E278" t="s">
-        <v>84</v>
       </c>
       <c r="F278" t="s">
         <v>22</v>
@@ -5208,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="B291" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="292" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5224,7 +5227,7 @@
         <v>2</v>
       </c>
       <c r="B293" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="294" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5256,15 +5259,15 @@
         <v>9</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="298" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A298" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B298" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B298" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="299" spans="1:7" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5297,7 +5300,7 @@
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A301" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B301">
         <v>1</v>
@@ -5312,12 +5315,12 @@
         <v>15</v>
       </c>
       <c r="G301" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A302" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B302">
         <v>0.56999999999999995</v>
@@ -5332,32 +5335,32 @@
         <v>18</v>
       </c>
       <c r="G302" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A303" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B303">
         <v>0.11</v>
       </c>
       <c r="C303" t="s">
+        <v>89</v>
+      </c>
+      <c r="D303" t="s">
+        <v>6</v>
+      </c>
+      <c r="F303" t="s">
+        <v>18</v>
+      </c>
+      <c r="G303" t="s">
         <v>90</v>
-      </c>
-      <c r="D303" t="s">
-        <v>6</v>
-      </c>
-      <c r="F303" t="s">
-        <v>18</v>
-      </c>
-      <c r="G303" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A304" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B304">
         <v>0.31</v>
@@ -5372,7 +5375,7 @@
         <v>18</v>
       </c>
       <c r="G304" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="306" spans="1:7" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5380,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="B306" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="307" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5396,7 +5399,7 @@
         <v>2</v>
       </c>
       <c r="B308" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="309" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -5428,15 +5431,15 @@
         <v>9</v>
       </c>
       <c r="B312" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="313" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A313" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B313" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="B313" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="314" spans="1:7" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -5469,7 +5472,7 @@
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A316" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B316">
         <v>1</v>
@@ -5484,12 +5487,12 @@
         <v>15</v>
       </c>
       <c r="G316" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A317" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B317" s="3">
         <v>4760</v>
@@ -5504,18 +5507,18 @@
         <v>18</v>
       </c>
       <c r="G317" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A318" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B318" s="3">
         <v>-9520</v>
       </c>
       <c r="C318" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D318" t="s">
         <v>6</v>
@@ -5524,12 +5527,12 @@
         <v>18</v>
       </c>
       <c r="G318" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A319" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B319" s="3">
         <v>4760</v>
@@ -5544,12 +5547,12 @@
         <v>18</v>
       </c>
       <c r="G319" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A320" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B320" s="3">
         <v>26700</v>
@@ -5564,12 +5567,12 @@
         <v>18</v>
       </c>
       <c r="G320" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A321" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B321" s="3">
         <v>6600</v>
@@ -5584,7 +5587,7 @@
         <v>18</v>
       </c>
       <c r="G321" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="324" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>